<commit_message>
Update Electricity Rate Plan.xlsx
</commit_message>
<xml_diff>
--- a/decarbonize/components/electricity/Electricity Rate Plan.xlsx
+++ b/decarbonize/components/electricity/Electricity Rate Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11606\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6AAE8E-7030-4CEE-9C30-A9F9C2F49734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C71FAAF-450F-416C-8057-93E1F2AE2C95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PG&amp;E Service Area" sheetId="4" r:id="rId1"/>
@@ -3638,13 +3638,13 @@
     <t>Customer Charge Rate</t>
   </si>
   <si>
-    <t>Customer Charge Phase</t>
-  </si>
-  <si>
     <t>Poly</t>
   </si>
   <si>
     <t>Single</t>
+  </si>
+  <si>
+    <t>Phase</t>
   </si>
 </sst>
 </file>
@@ -3832,7 +3832,7 @@
     <tableColumn id="6" xr3:uid="{94EB86F2-F482-4CBE-806C-8D97D13A25E7}" name="Peak Start Time"/>
     <tableColumn id="7" xr3:uid="{6BB546D3-5E89-4D2F-9DF8-4A6ED642F53E}" name="Peak End Time"/>
     <tableColumn id="8" xr3:uid="{D5557896-F71D-4CC5-83C0-4B0B735C716B}" name="Energy Rate"/>
-    <tableColumn id="9" xr3:uid="{F366E48E-3EAD-4BB4-930E-AE9C9B1D797B}" name="Customer Charge Phase"/>
+    <tableColumn id="9" xr3:uid="{F366E48E-3EAD-4BB4-930E-AE9C9B1D797B}" name="Phase"/>
     <tableColumn id="10" xr3:uid="{4C8D4DCE-7867-4EAB-BF6A-F57DF7F83FB1}" name="Customer Charge Rate"/>
     <tableColumn id="11" xr3:uid="{D69D3E4A-22AC-40B8-A09A-EC55B4C25C3D}" name="Day"/>
   </tableColumns>
@@ -3849,7 +3849,7 @@
     <tableColumn id="3" xr3:uid="{E45491CD-B1C6-40F5-B2B7-B604E35BB85B}" name="Bundling"/>
     <tableColumn id="4" xr3:uid="{8A9815F9-C665-49B7-A662-C70A8E79633D}" name="Season"/>
     <tableColumn id="5" xr3:uid="{95F70520-D039-4FD5-B9AB-803CA753ABA9}" name="Type"/>
-    <tableColumn id="6" xr3:uid="{E2DACF2F-882A-48C7-9504-1E861CAF6D60}" name="Customer Charge Phase"/>
+    <tableColumn id="6" xr3:uid="{E2DACF2F-882A-48C7-9504-1E861CAF6D60}" name="Phase"/>
     <tableColumn id="7" xr3:uid="{16D8FD66-8134-435B-B886-594D6CD986A8}" name="Customer Charge Rate"/>
     <tableColumn id="8" xr3:uid="{17BC28BB-1547-4E43-B886-AD9DCAC3DCED}" name="Peak Start Time"/>
     <tableColumn id="9" xr3:uid="{5285F431-A90E-477B-A233-960DF0E507EA}" name="Peak End Time"/>
@@ -20111,7 +20111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7BF5F5-9B64-444F-8807-74F4F2EE40E4}">
   <dimension ref="A1:J409"/>
   <sheetViews>
-    <sheetView topLeftCell="A382" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -32840,8 +32840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFE5BC1-8421-49E5-ABE6-1D57EBB6A57D}">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32885,7 +32885,7 @@
         <v>894</v>
       </c>
       <c r="I1" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="J1" t="s">
         <v>895</v>
@@ -32920,7 +32920,7 @@
         <v>0.46845999999999999</v>
       </c>
       <c r="I2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J2">
         <v>0.32854</v>
@@ -32955,7 +32955,7 @@
         <v>0.41148000000000001</v>
       </c>
       <c r="I3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J3">
         <v>0.32854</v>
@@ -32990,7 +32990,7 @@
         <v>0.46845999999999999</v>
       </c>
       <c r="I4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J4">
         <v>0.82135999999999998</v>
@@ -33025,7 +33025,7 @@
         <v>0.41148000000000001</v>
       </c>
       <c r="I5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J5">
         <v>0.82135999999999998</v>
@@ -33060,7 +33060,7 @@
         <v>0.4713</v>
       </c>
       <c r="I6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J6">
         <v>0.32854</v>
@@ -33095,7 +33095,7 @@
         <v>0.4713</v>
       </c>
       <c r="I7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J7">
         <v>0.32854</v>
@@ -33130,7 +33130,7 @@
         <v>0.4713</v>
       </c>
       <c r="I8" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J8">
         <v>0.32854</v>
@@ -33165,7 +33165,7 @@
         <v>0.4466</v>
       </c>
       <c r="I9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J9">
         <v>0.32854</v>
@@ -33200,7 +33200,7 @@
         <v>0.4466</v>
       </c>
       <c r="I10" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J10">
         <v>0.32854</v>
@@ -33235,7 +33235,7 @@
         <v>0.42371999999999999</v>
       </c>
       <c r="I11" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J11">
         <v>0.32854</v>
@@ -33270,7 +33270,7 @@
         <v>0.42314000000000002</v>
       </c>
       <c r="I12" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J12">
         <v>0.32854</v>
@@ -33305,7 +33305,7 @@
         <v>0.42314000000000002</v>
       </c>
       <c r="I13" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J13">
         <v>0.32854</v>
@@ -33340,7 +33340,7 @@
         <v>0.4713</v>
       </c>
       <c r="I14" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J14">
         <v>0.82135999999999998</v>
@@ -33375,7 +33375,7 @@
         <v>0.4713</v>
       </c>
       <c r="I15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J15">
         <v>0.82135999999999998</v>
@@ -33410,7 +33410,7 @@
         <v>0.4713</v>
       </c>
       <c r="I16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J16">
         <v>0.82135999999999998</v>
@@ -33445,7 +33445,7 @@
         <v>0.4466</v>
       </c>
       <c r="I17" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J17">
         <v>0.82135999999999998</v>
@@ -33480,7 +33480,7 @@
         <v>0.4466</v>
       </c>
       <c r="I18" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J18">
         <v>0.82135999999999998</v>
@@ -33515,7 +33515,7 @@
         <v>0.42371999999999999</v>
       </c>
       <c r="I19" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J19">
         <v>0.82135999999999998</v>
@@ -33550,7 +33550,7 @@
         <v>0.42314000000000002</v>
       </c>
       <c r="I20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J20">
         <v>0.82135999999999998</v>
@@ -33585,7 +33585,7 @@
         <v>0.42314000000000002</v>
       </c>
       <c r="I21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J21">
         <v>0.82135999999999998</v>
@@ -33620,7 +33620,7 @@
         <v>0.51710999999999996</v>
       </c>
       <c r="I22" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J22">
         <v>0.32854</v>
@@ -33655,7 +33655,7 @@
         <v>0.46788000000000002</v>
       </c>
       <c r="I23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J23">
         <v>0.32854</v>
@@ -33690,7 +33690,7 @@
         <v>0.46788000000000002</v>
       </c>
       <c r="I24" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J24">
         <v>0.32854</v>
@@ -33725,7 +33725,7 @@
         <v>0.44707000000000002</v>
       </c>
       <c r="I25" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J25">
         <v>0.32854</v>
@@ -33760,7 +33760,7 @@
         <v>0.44169000000000003</v>
       </c>
       <c r="I26" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J26">
         <v>0.32854</v>
@@ -33795,7 +33795,7 @@
         <v>0.40915000000000001</v>
       </c>
       <c r="I27" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J27">
         <v>0.32854</v>
@@ -33830,7 +33830,7 @@
         <v>0.42557</v>
       </c>
       <c r="I28" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J28">
         <v>0.32854</v>
@@ -33865,7 +33865,7 @@
         <v>0.51710999999999996</v>
       </c>
       <c r="I29" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J29">
         <v>0.82135999999999998</v>
@@ -33900,7 +33900,7 @@
         <v>0.46788000000000002</v>
       </c>
       <c r="I30" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J30">
         <v>0.82135999999999998</v>
@@ -33935,7 +33935,7 @@
         <v>0.46788000000000002</v>
       </c>
       <c r="I31" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J31">
         <v>0.82135999999999998</v>
@@ -33970,7 +33970,7 @@
         <v>0.44707000000000002</v>
       </c>
       <c r="I32" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J32">
         <v>0.82135999999999998</v>
@@ -34005,7 +34005,7 @@
         <v>0.44169000000000003</v>
       </c>
       <c r="I33" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J33">
         <v>0.82135999999999998</v>
@@ -34040,7 +34040,7 @@
         <v>0.40915000000000001</v>
       </c>
       <c r="I34" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J34">
         <v>0.82135999999999998</v>
@@ -34075,7 +34075,7 @@
         <v>0.42557</v>
       </c>
       <c r="I35" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J35">
         <v>0.82135999999999998</v>
@@ -34110,7 +34110,7 @@
         <v>0.54356000000000004</v>
       </c>
       <c r="I36" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J36">
         <v>0.32854</v>
@@ -34145,7 +34145,7 @@
         <v>0.40226000000000001</v>
       </c>
       <c r="I37" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J37">
         <v>0.32854</v>
@@ -34180,7 +34180,7 @@
         <v>0.40226000000000001</v>
       </c>
       <c r="I38" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J38">
         <v>0.32854</v>
@@ -34215,7 +34215,7 @@
         <v>0.35493000000000002</v>
       </c>
       <c r="I39" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J39">
         <v>0.32854</v>
@@ -34250,7 +34250,7 @@
         <v>0.44561000000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J40">
         <v>0.32854</v>
@@ -34285,7 +34285,7 @@
         <v>0.41660999999999998</v>
       </c>
       <c r="I41" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J41">
         <v>0.32854</v>
@@ -34320,7 +34320,7 @@
         <v>0.41660999999999998</v>
       </c>
       <c r="I42" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J42">
         <v>0.32854</v>
@@ -34355,7 +34355,7 @@
         <v>0.31064000000000003</v>
       </c>
       <c r="I43" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J43">
         <v>0.32854</v>
@@ -34390,7 +34390,7 @@
         <v>0.32706000000000002</v>
       </c>
       <c r="I44" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J44">
         <v>0.32854</v>
@@ -34425,7 +34425,7 @@
         <v>0.54356000000000004</v>
       </c>
       <c r="I45" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J45">
         <v>0.82135999999999998</v>
@@ -34460,7 +34460,7 @@
         <v>0.40226000000000001</v>
       </c>
       <c r="I46" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J46">
         <v>0.82135999999999998</v>
@@ -34495,7 +34495,7 @@
         <v>0.40226000000000001</v>
       </c>
       <c r="I47" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J47">
         <v>0.82135999999999998</v>
@@ -34530,7 +34530,7 @@
         <v>0.35493000000000002</v>
       </c>
       <c r="I48" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J48">
         <v>0.82135999999999998</v>
@@ -34565,7 +34565,7 @@
         <v>0.44561000000000001</v>
       </c>
       <c r="I49" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J49">
         <v>0.82135999999999998</v>
@@ -34600,7 +34600,7 @@
         <v>0.41660999999999998</v>
       </c>
       <c r="I50" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J50">
         <v>0.82135999999999998</v>
@@ -34635,7 +34635,7 @@
         <v>0.41660999999999998</v>
       </c>
       <c r="I51" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J51">
         <v>0.82135999999999998</v>
@@ -34670,7 +34670,7 @@
         <v>0.31064000000000003</v>
       </c>
       <c r="I52" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J52">
         <v>0.82135999999999998</v>
@@ -34705,7 +34705,7 @@
         <v>0.32706000000000002</v>
       </c>
       <c r="I53" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J53">
         <v>0.82135999999999998</v>
@@ -34740,7 +34740,7 @@
         <v>0.69103000000000003</v>
       </c>
       <c r="I54" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J54">
         <v>0.32854</v>
@@ -34775,7 +34775,7 @@
         <v>0.43340000000000001</v>
       </c>
       <c r="I55" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J55">
         <v>0.32854</v>
@@ -34810,7 +34810,7 @@
         <v>0.44434000000000001</v>
       </c>
       <c r="I56" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J56">
         <v>0.32854</v>
@@ -34845,7 +34845,7 @@
         <v>0.36465999999999998</v>
       </c>
       <c r="I57" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J57">
         <v>0.32854</v>
@@ -34880,7 +34880,7 @@
         <v>0.40073999999999999</v>
       </c>
       <c r="I58" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="J58">
         <v>0.32854</v>
@@ -34915,7 +34915,7 @@
         <v>0.69103000000000003</v>
       </c>
       <c r="I59" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J59">
         <v>0.82135999999999998</v>
@@ -34950,7 +34950,7 @@
         <v>0.43340000000000001</v>
       </c>
       <c r="I60" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J60">
         <v>0.82135999999999998</v>
@@ -34985,7 +34985,7 @@
         <v>0.44434000000000001</v>
       </c>
       <c r="I61" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J61">
         <v>0.82135999999999998</v>
@@ -35020,7 +35020,7 @@
         <v>0.36465999999999998</v>
       </c>
       <c r="I62" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J62">
         <v>0.82135999999999998</v>
@@ -35055,7 +35055,7 @@
         <v>0.40073999999999999</v>
       </c>
       <c r="I63" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J63">
         <v>0.82135999999999998</v>
@@ -37913,8 +37913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB37B77-99CE-44F2-93F7-0E4FB0E2ED7E}">
   <dimension ref="A1:Z144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37963,7 +37963,7 @@
         <v>849</v>
       </c>
       <c r="F1" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="G1" t="s">
         <v>895</v>
@@ -38043,7 +38043,7 @@
         <v>856</v>
       </c>
       <c r="F2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G2">
         <v>0.32854</v>
@@ -38123,7 +38123,7 @@
         <v>856</v>
       </c>
       <c r="F3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G3">
         <v>0.32854</v>
@@ -38203,7 +38203,7 @@
         <v>856</v>
       </c>
       <c r="F4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G4">
         <v>0.82135999999999998</v>
@@ -38283,7 +38283,7 @@
         <v>856</v>
       </c>
       <c r="F5" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G5">
         <v>0.82135999999999998</v>
@@ -38363,7 +38363,7 @@
         <v>850</v>
       </c>
       <c r="F6" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G6">
         <v>0.32854</v>
@@ -38443,7 +38443,7 @@
         <v>857</v>
       </c>
       <c r="F7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G7">
         <v>0.32854</v>
@@ -38523,7 +38523,7 @@
         <v>857</v>
       </c>
       <c r="F8" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G8">
         <v>0.32854</v>
@@ -38603,7 +38603,7 @@
         <v>851</v>
       </c>
       <c r="F9" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G9">
         <v>0.32854</v>
@@ -38683,7 +38683,7 @@
         <v>851</v>
       </c>
       <c r="F10" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G10">
         <v>0.32854</v>
@@ -38763,7 +38763,7 @@
         <v>857</v>
       </c>
       <c r="F11" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G11">
         <v>0.32854</v>
@@ -38843,7 +38843,7 @@
         <v>851</v>
       </c>
       <c r="F12" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G12">
         <v>0.32854</v>
@@ -38923,7 +38923,7 @@
         <v>851</v>
       </c>
       <c r="F13" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G13">
         <v>0.32854</v>
@@ -39003,7 +39003,7 @@
         <v>850</v>
       </c>
       <c r="F14" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G14">
         <v>0.82135999999999998</v>
@@ -39083,7 +39083,7 @@
         <v>857</v>
       </c>
       <c r="F15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G15">
         <v>0.82135999999999998</v>
@@ -39163,7 +39163,7 @@
         <v>857</v>
       </c>
       <c r="F16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G16">
         <v>0.82135999999999998</v>
@@ -39243,7 +39243,7 @@
         <v>851</v>
       </c>
       <c r="F17" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G17">
         <v>0.82135999999999998</v>
@@ -39323,7 +39323,7 @@
         <v>851</v>
       </c>
       <c r="F18" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G18">
         <v>0.82135999999999998</v>
@@ -39403,7 +39403,7 @@
         <v>857</v>
       </c>
       <c r="F19" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G19">
         <v>0.82135999999999998</v>
@@ -39483,7 +39483,7 @@
         <v>851</v>
       </c>
       <c r="F20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G20">
         <v>0.82135999999999998</v>
@@ -39563,7 +39563,7 @@
         <v>851</v>
       </c>
       <c r="F21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G21">
         <v>0.82135999999999998</v>
@@ -39643,7 +39643,7 @@
         <v>850</v>
       </c>
       <c r="F22" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G22">
         <v>0.32854</v>
@@ -39723,7 +39723,7 @@
         <v>857</v>
       </c>
       <c r="F23" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G23">
         <v>0.32854</v>
@@ -39803,7 +39803,7 @@
         <v>857</v>
       </c>
       <c r="F24" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G24">
         <v>0.32854</v>
@@ -39883,7 +39883,7 @@
         <v>851</v>
       </c>
       <c r="F25" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G25">
         <v>0.32854</v>
@@ -39963,7 +39963,7 @@
         <v>850</v>
       </c>
       <c r="F26" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G26">
         <v>0.32854</v>
@@ -40043,7 +40043,7 @@
         <v>860</v>
       </c>
       <c r="F27" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G27">
         <v>0.32854</v>
@@ -40123,7 +40123,7 @@
         <v>851</v>
       </c>
       <c r="F28" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G28">
         <v>0.32854</v>
@@ -40203,7 +40203,7 @@
         <v>850</v>
       </c>
       <c r="F29" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G29">
         <v>0.82135999999999998</v>
@@ -40283,7 +40283,7 @@
         <v>857</v>
       </c>
       <c r="F30" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G30">
         <v>0.82135999999999998</v>
@@ -40363,7 +40363,7 @@
         <v>857</v>
       </c>
       <c r="F31" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G31">
         <v>0.82135999999999998</v>
@@ -40443,7 +40443,7 @@
         <v>851</v>
       </c>
       <c r="F32" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G32">
         <v>0.82135999999999998</v>
@@ -40523,7 +40523,7 @@
         <v>850</v>
       </c>
       <c r="F33" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G33">
         <v>0.82135999999999998</v>
@@ -40603,7 +40603,7 @@
         <v>860</v>
       </c>
       <c r="F34" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G34">
         <v>0.82135999999999998</v>
@@ -40683,7 +40683,7 @@
         <v>851</v>
       </c>
       <c r="F35" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G35">
         <v>0.82135999999999998</v>
@@ -40763,7 +40763,7 @@
         <v>850</v>
       </c>
       <c r="F36" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G36">
         <v>0.32854</v>
@@ -40843,7 +40843,7 @@
         <v>857</v>
       </c>
       <c r="F37" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G37">
         <v>0.32854</v>
@@ -40923,7 +40923,7 @@
         <v>857</v>
       </c>
       <c r="F38" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G38">
         <v>0.32854</v>
@@ -41003,7 +41003,7 @@
         <v>851</v>
       </c>
       <c r="F39" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G39">
         <v>0.32854</v>
@@ -41083,7 +41083,7 @@
         <v>850</v>
       </c>
       <c r="F40" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G40">
         <v>0.32854</v>
@@ -41163,7 +41163,7 @@
         <v>857</v>
       </c>
       <c r="F41" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G41">
         <v>0.32854</v>
@@ -41243,7 +41243,7 @@
         <v>857</v>
       </c>
       <c r="F42" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G42">
         <v>0.32854</v>
@@ -41323,7 +41323,7 @@
         <v>860</v>
       </c>
       <c r="F43" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G43">
         <v>0.32854</v>
@@ -41403,7 +41403,7 @@
         <v>851</v>
       </c>
       <c r="F44" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G44">
         <v>0.32854</v>
@@ -41483,7 +41483,7 @@
         <v>850</v>
       </c>
       <c r="F45" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G45">
         <v>0.82135999999999998</v>
@@ -41563,7 +41563,7 @@
         <v>857</v>
       </c>
       <c r="F46" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G46">
         <v>0.82135999999999998</v>
@@ -41643,7 +41643,7 @@
         <v>857</v>
       </c>
       <c r="F47" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G47">
         <v>0.82135999999999998</v>
@@ -41723,7 +41723,7 @@
         <v>851</v>
       </c>
       <c r="F48" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G48">
         <v>0.82135999999999998</v>
@@ -41803,7 +41803,7 @@
         <v>850</v>
       </c>
       <c r="F49" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G49">
         <v>0.82135999999999998</v>
@@ -41883,7 +41883,7 @@
         <v>857</v>
       </c>
       <c r="F50" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G50">
         <v>0.82135999999999998</v>
@@ -41963,7 +41963,7 @@
         <v>857</v>
       </c>
       <c r="F51" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G51">
         <v>0.82135999999999998</v>
@@ -42043,7 +42043,7 @@
         <v>860</v>
       </c>
       <c r="F52" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G52">
         <v>0.82135999999999998</v>
@@ -42123,7 +42123,7 @@
         <v>851</v>
       </c>
       <c r="F53" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G53">
         <v>0.82135999999999998</v>
@@ -42203,7 +42203,7 @@
         <v>850</v>
       </c>
       <c r="F54" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G54">
         <v>0.32854</v>
@@ -42283,7 +42283,7 @@
         <v>851</v>
       </c>
       <c r="F55" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G55">
         <v>0.32854</v>
@@ -42363,7 +42363,7 @@
         <v>850</v>
       </c>
       <c r="F56" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G56">
         <v>0.32854</v>
@@ -42443,7 +42443,7 @@
         <v>860</v>
       </c>
       <c r="F57" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G57">
         <v>0.32854</v>
@@ -42523,7 +42523,7 @@
         <v>851</v>
       </c>
       <c r="F58" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G58">
         <v>0.32854</v>
@@ -42603,7 +42603,7 @@
         <v>850</v>
       </c>
       <c r="F59" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G59">
         <v>0.82135999999999998</v>
@@ -42683,7 +42683,7 @@
         <v>851</v>
       </c>
       <c r="F60" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G60">
         <v>0.82135999999999998</v>
@@ -42763,7 +42763,7 @@
         <v>850</v>
       </c>
       <c r="F61" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G61">
         <v>0.82135999999999998</v>
@@ -42843,7 +42843,7 @@
         <v>860</v>
       </c>
       <c r="F62" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G62">
         <v>0.82135999999999998</v>
@@ -42923,7 +42923,7 @@
         <v>851</v>
       </c>
       <c r="F63" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G63">
         <v>0.82135999999999998</v>

</xml_diff>